<commit_message>
Content transferred, intial version
</commit_message>
<xml_diff>
--- a/docs/00b-basics/pie-chart-overview.xlsx
+++ b/docs/00b-basics/pie-chart-overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Documents/developer/github_isaqb/advanced-template/docs/01-basics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\isaqb\curriculum-arceval\docs\00b-basics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182FF1B4-E76D-1644-8110-6BB9862D395E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD012E0-5F3A-4754-8A46-A7DB89C116A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="460" windowWidth="24560" windowHeight="15540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="28800" windowHeight="15290" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DE-Grafik" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -47,24 +49,6 @@
     <t>Gesamt</t>
   </si>
   <si>
-    <t>Thema mit Einleitung</t>
-  </si>
-  <si>
-    <t>Thema über xz</t>
-  </si>
-  <si>
-    <t>Thema mit viel Theorie</t>
-  </si>
-  <si>
-    <t>Thema mit xy und Beispiel</t>
-  </si>
-  <si>
-    <t>Thema mit abc und d</t>
-  </si>
-  <si>
-    <t>Thema mit Abschlussbeispiel</t>
-  </si>
-  <si>
     <t>Introduction</t>
   </si>
   <si>
@@ -82,12 +66,30 @@
   <si>
     <t>final example</t>
   </si>
+  <si>
+    <t>Grundbegriffe von Software-Architekturbewertung</t>
+  </si>
+  <si>
+    <t>Anforderungen in der Architekturbewertung</t>
+  </si>
+  <si>
+    <t>Bewertungsworkshop</t>
+  </si>
+  <si>
+    <t>Nacharbeit und Ergebnisverwertung</t>
+  </si>
+  <si>
+    <t>Bewertung bestehender System(-teil)e</t>
+  </si>
+  <si>
+    <t>Beispiele für die Bewertung von Software-Architekturen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,7 +128,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -144,7 +146,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -310,29 +312,8 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.82861803157886E-2"/>
-                  <c:y val="-5.3475002371691498E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="1.0442785857776435E-2"/>
-                  <c:y val="-3.2186462384972997E-2"/>
+                  <c:x val="-1.8824882412863446E-2"/>
+                  <c:y val="-5.3475002371691512E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -345,8 +326,36 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.20891240362272728"/>
-                      <c:h val="0.19607003390775066"/>
+                      <c:w val="0.2386991527135135"/>
+                      <c:h val="0.15032862972307881"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.8482356872571655E-3"/>
+                  <c:y val="2.9303826456740516E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.27285648033675614"/>
+                      <c:h val="0.1960700569117228"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -379,22 +388,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Thema mit Einleitung</c:v>
+                  <c:v>Grundbegriffe von Software-Architekturbewertung</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Thema über xz</c:v>
+                  <c:v>Anforderungen in der Architekturbewertung</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Thema mit viel Theorie</c:v>
+                  <c:v>Bewertungsworkshop</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Thema mit xy und Beispiel</c:v>
+                  <c:v>Nacharbeit und Ergebnisverwertung</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Thema mit abc und d</c:v>
+                  <c:v>Bewertung bestehender System(-teil)e</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Thema mit Abschlussbeispiel</c:v>
+                  <c:v>Beispiele für die Bewertung von Software-Architekturen</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -406,22 +415,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>180</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>120</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>180</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>210</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>120</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -477,7 +486,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -806,14 +815,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>160234</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>50801</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1208,70 +1217,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="42" style="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>9</v>
       </c>
       <c r="B1" s="1">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>10</v>
       </c>
       <c r="B2" s="1">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>11</v>
       </c>
       <c r="B3" s="1">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>12</v>
       </c>
       <c r="B4" s="1">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>13</v>
       </c>
       <c r="B5" s="1">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>14</v>
       </c>
       <c r="B6" s="1">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="B7" s="1">
         <f>SUM(B1:B6)</f>
-        <v>960</v>
+        <v>840</v>
       </c>
     </row>
   </sheetData>
@@ -1289,7 +1298,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="34.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1"/>
@@ -1297,55 +1306,55 @@
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1">
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="B7" s="1">
         <f>SUM(B1:B6)</f>
         <v>960</v>
@@ -1361,16 +1370,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="249" zoomScaleNormal="249" zoomScalePageLayoutView="249" workbookViewId="0">
+    <sheetView zoomScale="249" zoomScaleNormal="249" zoomScalePageLayoutView="249" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1381,7 +1390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1393,7 +1402,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1408,7 +1417,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1423,7 +1432,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1438,7 +1447,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1453,7 +1462,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1468,7 +1477,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1483,7 +1492,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="D10" s="1">
         <f>SUM(D2:D8)</f>
         <v>960</v>

</xml_diff>